<commit_message>
(+) added Reservoir files in package (*) rearranged the methods in Controller and service (+) added new file to decide rest end points (*) formatting of the other files
</commit_message>
<xml_diff>
--- a/Documentation/TraceabilityMatrix.xlsx
+++ b/Documentation/TraceabilityMatrix.xlsx
@@ -5,18 +5,19 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS\SEM 1\SCS\Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36F0262-AD75-4366-A69E-EE077CB58D8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A079C05F-9B9C-4AD0-93DE-53789274272B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="459" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="459" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="5" r:id="rId1"/>
     <sheet name="RTM" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="92512" iterateDelta="1E-4" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -108,9 +109,6 @@
     <t>Functional Requirement</t>
   </si>
   <si>
-    <t>Test Cased ID #</t>
-  </si>
-  <si>
     <t>Test Case Description</t>
   </si>
   <si>
@@ -336,6 +334,9 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>Test Case ID #</t>
   </si>
 </sst>
 </file>
@@ -1056,16 +1057,16 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="91.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="91.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
@@ -1082,7 +1083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1099,7 +1100,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1110,15 +1111,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D5" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>23</v>
       </c>
@@ -1126,9 +1127,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>12</v>
@@ -1151,25 +1152,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="71.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="71.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1180,24 +1181,24 @@
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
     </row>
-    <row r="3" spans="1:9" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="23"/>
       <c r="C3" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="23"/>
       <c r="F3" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
       <c r="I3" s="23"/>
     </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" s="4" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
@@ -1214,19 +1215,19 @@
         <v>0</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -1234,130 +1235,130 @@
         <v>21</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>41</v>
-      </c>
       <c r="H7" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="14" t="s">
-        <v>43</v>
-      </c>
       <c r="H8" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -1368,47 +1369,47 @@
       <c r="H12" s="12"/>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>53</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -1419,64 +1420,64 @@
       <c r="H15" s="12"/>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="14" t="s">
-        <v>64</v>
-      </c>
       <c r="H18" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -1487,64 +1488,64 @@
       <c r="H19" s="12"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="14" t="s">
-        <v>69</v>
-      </c>
       <c r="H20" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G21" s="14" t="s">
-        <v>71</v>
-      </c>
       <c r="H21" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="G22" s="14" t="s">
-        <v>73</v>
-      </c>
       <c r="H22" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
@@ -1555,7 +1556,7 @@
       <c r="H23" s="12"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -1566,7 +1567,7 @@
       <c r="H24" s="12"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>3</v>
       </c>
@@ -1574,43 +1575,43 @@
         <v>22</v>
       </c>
       <c r="C25" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="F25" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G25" s="14" t="s">
-        <v>80</v>
-      </c>
       <c r="H25" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="G26" s="14" t="s">
-        <v>82</v>
-      </c>
       <c r="H26" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="12"/>
@@ -1621,64 +1622,64 @@
       <c r="H27" s="12"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="E28" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F28" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="G28" s="12" t="s">
-        <v>85</v>
-      </c>
       <c r="H28" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
       <c r="F29" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="F30" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="G30" s="14" t="s">
-        <v>89</v>
-      </c>
       <c r="H30" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -1689,7 +1690,7 @@
       <c r="H31" s="12"/>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -1700,81 +1701,81 @@
       <c r="H32" s="12"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" s="12" t="s">
+      <c r="D33" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="E33" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="E33" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="F33" s="12" t="s">
+      <c r="G33" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="G33" s="12" t="s">
-        <v>95</v>
-      </c>
       <c r="H33" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
       <c r="F34" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G34" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="G34" s="12" t="s">
-        <v>97</v>
-      </c>
       <c r="H34" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
       <c r="F35" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G35" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="G35" s="12" t="s">
-        <v>99</v>
-      </c>
       <c r="H35" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
       <c r="E36" s="17"/>
       <c r="F36" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="G36" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="G36" s="18" t="s">
-        <v>101</v>
-      </c>
       <c r="H36" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I36" s="19"/>
     </row>

</xml_diff>